<commit_message>
Insert data from Excel document API
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/sample.xlsx
+++ b/src/main/resources/documents/sample.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="TAB1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -180,7 +180,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.53"/>

</xml_diff>